<commit_message>
All but one path test passes on Board class
</commit_message>
<xml_diff>
--- a/clueLayout(for part 2).xlsx
+++ b/clueLayout(for part 2).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -108,8 +108,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +378,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -412,6 +413,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -587,16 +589,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="18.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75" customHeight="1">
+    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -671,7 +673,7 @@
       </c>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" ht="18.75" customHeight="1">
+    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -747,7 +749,7 @@
       </c>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="18.75" customHeight="1">
+    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -823,7 +825,7 @@
       </c>
       <c r="Z3" s="6"/>
     </row>
-    <row r="4" spans="1:26" ht="18.75" customHeight="1">
+    <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -899,7 +901,7 @@
       </c>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="18.75" customHeight="1">
+    <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -975,7 +977,7 @@
       </c>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" ht="18.75" customHeight="1">
+    <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1051,7 +1053,7 @@
       </c>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="18.75" customHeight="1">
+    <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1127,7 +1129,7 @@
       </c>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" ht="18.75" customHeight="1">
+    <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -1203,7 +1205,7 @@
       </c>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="18.75" customHeight="1">
+    <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
@@ -1279,7 +1281,7 @@
       </c>
       <c r="Z9" s="7"/>
     </row>
-    <row r="10" spans="1:26" ht="18.75" customHeight="1">
+    <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1355,7 +1357,7 @@
       </c>
       <c r="Z10" s="7"/>
     </row>
-    <row r="11" spans="1:26" ht="18.75" customHeight="1">
+    <row r="11" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1431,7 +1433,7 @@
       </c>
       <c r="Z11" s="7"/>
     </row>
-    <row r="12" spans="1:26" ht="18.75" customHeight="1">
+    <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1507,7 +1509,7 @@
       </c>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26" ht="18.75" customHeight="1">
+    <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1582,7 +1584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="18.75" customHeight="1">
+    <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="18.75" customHeight="1">
+    <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
@@ -1732,7 +1734,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="18.75" customHeight="1">
+    <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -1807,7 +1809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="18.75" customHeight="1">
+    <row r="17" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>5</v>
       </c>
@@ -1882,7 +1884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="18.75" customHeight="1">
+    <row r="18" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -1957,7 +1959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="18.75" customHeight="1">
+    <row r="19" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -2032,7 +2034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="18.75" customHeight="1">
+    <row r="20" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -2107,7 +2109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="18.75" customHeight="1">
+    <row r="21" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -2182,7 +2184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="18.75" customHeight="1">
+    <row r="22" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -2257,7 +2259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="18.75" customHeight="1">
+    <row r="23" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -2351,54 +2353,54 @@
       </c>
       <c r="X23" s="1"/>
     </row>
-    <row r="24" spans="1:24" ht="18.75" customHeight="1">
+    <row r="24" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="18.75" customHeight="1">
+    <row r="25" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="18.75" customHeight="1">
+    <row r="26" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="18.75" customHeight="1">
+    <row r="27" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="18.75" customHeight="1">
+    <row r="28" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="18.75" customHeight="1">
+    <row r="29" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="18.75" customHeight="1">
+    <row r="30" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="18.75" customHeight="1">
+    <row r="31" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
       <c r="B31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="18.75" customHeight="1">
+    <row r="32" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" t="s">
         <v>27</v>
@@ -2411,24 +2413,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>